<commit_message>
feat: working program with generating the keys
</commit_message>
<xml_diff>
--- a/output/fw8ben.xlsx
+++ b/output/fw8ben.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,6 +429,16 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Custom Label</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Value</t>
         </is>
       </c>
@@ -439,7 +449,21 @@
           <t>f_1[0]</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NAME_OF_INDIVIDUAL</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Ashok Rohidas Modhave</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -447,7 +471,21 @@
           <t>f_2[0]</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>COUNTRY_OF_RESIDENCE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -455,7 +493,17 @@
           <t>f_3[0]</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Aundh, Pune</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -463,7 +511,17 @@
           <t>f_4[0]</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Pune, Maharashtra 411011</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -471,7 +529,17 @@
           <t>f_5[0]</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -479,7 +547,13 @@
           <t>f_6[0]</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -487,7 +561,13 @@
           <t>f_7[0]</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -495,7 +575,13 @@
           <t>f_8[0]</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -503,7 +589,17 @@
           <t>f_9[0]</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>123-433-112</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -511,7 +607,13 @@
           <t>f_10[0]</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -521,6 +623,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>checkbox</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>Unchecked</t>
         </is>
       </c>
@@ -531,7 +639,17 @@
           <t>f_11[0]</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -539,7 +657,17 @@
           <t>f_12[0]</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>03-01-1991</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -547,7 +675,17 @@
           <t>f_13[0]</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -555,7 +693,13 @@
           <t>f_14[0]</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -563,7 +707,13 @@
           <t>f_15[0]</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -571,7 +721,13 @@
           <t>f_16[0]</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -579,7 +735,13 @@
           <t>f_17[0]</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -587,7 +749,13 @@
           <t>f_18[0]</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -597,7 +765,13 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Unchecked</t>
+          <t>checkbox</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Checked</t>
         </is>
       </c>
     </row>
@@ -607,7 +781,13 @@
           <t>f_20[0]</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -615,7 +795,17 @@
           <t>Date[0]</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>08-13-2024</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -623,7 +813,17 @@
           <t>f_21[0]</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Ashok Modhave</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -631,7 +831,13 @@
           <t>Page1[0]</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -639,7 +845,13 @@
           <t>topmostSubform[0]</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>